<commit_message>
some channel position edits on excel file
</commit_message>
<xml_diff>
--- a/channel_105chRS1/Channel_location_105.xlsx
+++ b/channel_105chRS1/Channel_location_105.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandre.franco/Documents/GitHub/FNIRS_CMI/channel_105chRS1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC208F4A-C1FB-3C42-AFBD-DA9C79A4811E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4543A27-63AE-1546-8F07-F9760FDDF6F1}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="620" yWindow="880" windowWidth="10000" windowHeight="16620" xr2:uid="{E6BF8CDE-07C8-6D4D-B1D3-0A775E526C2F}"/>
+    <workbookView xWindow="620" yWindow="880" windowWidth="13040" windowHeight="18300" xr2:uid="{E6BF8CDE-07C8-6D4D-B1D3-0A775E526C2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
   <si>
     <t>Channel number</t>
   </si>
@@ -46,6 +46,21 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Left with H</t>
+  </si>
+  <si>
+    <t>Right With H</t>
+  </si>
+  <si>
+    <t>L no space</t>
+  </si>
+  <si>
+    <t>R no space</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -89,9 +104,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,27 +424,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61211ABD-1E82-8B4A-AFAD-B70B73058D38}">
-  <dimension ref="A1:F106"/>
+  <dimension ref="A1:BG106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B74" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B83" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F98" sqref="F98"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="4.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -441,11 +459,23 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -459,8 +489,22 @@
       <c r="F2">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H2">
+        <f>IF(B2=1,A2,"")</f>
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <f>IF(B2=1,F2,"")</f>
+        <v>4</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -474,8 +518,22 @@
       <c r="F3">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H3">
+        <f t="shared" ref="H3:H16" si="1">IF(B3=1,A3,"")</f>
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I16" si="2">IF(B3=1,F3,"")</f>
+        <v>3</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+      <c r="L3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -489,8 +547,22 @@
       <c r="F4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K4">
+        <v>5</v>
+      </c>
+      <c r="L4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -504,8 +576,22 @@
       <c r="F5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H5" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K5">
+        <v>8</v>
+      </c>
+      <c r="L5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -519,8 +605,22 @@
       <c r="F6">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="K6">
+        <v>10</v>
+      </c>
+      <c r="L6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -534,8 +634,22 @@
       <c r="F7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H7" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K7">
+        <v>13</v>
+      </c>
+      <c r="L7">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -549,8 +663,22 @@
       <c r="F8">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H8" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K8">
+        <v>14</v>
+      </c>
+      <c r="L8">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -564,8 +692,22 @@
       <c r="F9">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="K9">
+        <v>15</v>
+      </c>
+      <c r="L9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -579,8 +721,22 @@
       <c r="F10">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K10">
+        <v>19</v>
+      </c>
+      <c r="L10">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -594,8 +750,22 @@
       <c r="F11">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="K11">
+        <v>20</v>
+      </c>
+      <c r="L11">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -609,8 +779,22 @@
       <c r="F12" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K12">
+        <v>21</v>
+      </c>
+      <c r="L12">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -624,8 +808,22 @@
       <c r="F13">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H13" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K13">
+        <v>26</v>
+      </c>
+      <c r="L13">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -639,8 +837,22 @@
       <c r="F14">
         <v>18</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="K14">
+        <v>27</v>
+      </c>
+      <c r="L14">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -654,8 +866,22 @@
       <c r="F15">
         <v>17</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="K15">
+        <v>28</v>
+      </c>
+      <c r="L15">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -669,8 +895,22 @@
       <c r="F16">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H16">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="K16">
+        <v>29</v>
+      </c>
+      <c r="L16">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -684,8 +924,22 @@
       <c r="F17">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H17" t="str">
+        <f t="shared" ref="H17:H80" si="3">IF(B17=1,A17,"")</f>
+        <v/>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" ref="I17:I80" si="4">IF(B17=1,F17,"")</f>
+        <v/>
+      </c>
+      <c r="K17">
+        <v>34</v>
+      </c>
+      <c r="L17">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -699,8 +953,22 @@
       <c r="F18">
         <v>14</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I18" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K18">
+        <v>35</v>
+      </c>
+      <c r="L18">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -714,8 +982,22 @@
       <c r="F19">
         <v>13</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H19" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K19">
+        <v>36</v>
+      </c>
+      <c r="L19">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -729,8 +1011,22 @@
       <c r="F20">
         <v>25</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H20">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="4"/>
+        <v>25</v>
+      </c>
+      <c r="K20">
+        <v>37</v>
+      </c>
+      <c r="L20">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -744,8 +1040,22 @@
       <c r="F21">
         <v>24</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H21">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="4"/>
+        <v>24</v>
+      </c>
+      <c r="K21">
+        <v>43</v>
+      </c>
+      <c r="L21">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -759,8 +1069,22 @@
       <c r="F22">
         <v>23</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H22">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="4"/>
+        <v>23</v>
+      </c>
+      <c r="K22">
+        <v>44</v>
+      </c>
+      <c r="L22">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -771,8 +1095,22 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H23" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I23" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K23">
+        <v>45</v>
+      </c>
+      <c r="L23">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -786,8 +1124,22 @@
       <c r="F24">
         <v>21</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H24" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I24" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K24">
+        <v>46</v>
+      </c>
+      <c r="L24">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -801,8 +1153,22 @@
       <c r="F25">
         <v>20</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H25" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I25" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K25">
+        <v>51</v>
+      </c>
+      <c r="L25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -816,8 +1182,22 @@
       <c r="F26">
         <v>19</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H26" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I26" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K26">
+        <v>52</v>
+      </c>
+      <c r="L26">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -831,8 +1211,22 @@
       <c r="F27">
         <v>33</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H27">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="4"/>
+        <v>33</v>
+      </c>
+      <c r="K27">
+        <v>53</v>
+      </c>
+      <c r="L27">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -846,8 +1240,22 @@
       <c r="F28">
         <v>32</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H28">
+        <f t="shared" si="3"/>
+        <v>27</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="4"/>
+        <v>32</v>
+      </c>
+      <c r="K28">
+        <v>54</v>
+      </c>
+      <c r="L28">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -861,8 +1269,22 @@
       <c r="F29">
         <v>31</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H29">
+        <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="4"/>
+        <v>31</v>
+      </c>
+      <c r="K29">
+        <v>60</v>
+      </c>
+      <c r="L29">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -876,8 +1298,22 @@
       <c r="F30">
         <v>30</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H30">
+        <f t="shared" si="3"/>
+        <v>29</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="K30">
+        <v>61</v>
+      </c>
+      <c r="L30">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -891,8 +1327,22 @@
       <c r="F31">
         <v>29</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H31" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I31" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K31">
+        <v>62</v>
+      </c>
+      <c r="L31">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -906,8 +1356,22 @@
       <c r="F32">
         <v>28</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H32" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I32" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K32">
+        <v>63</v>
+      </c>
+      <c r="L32">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -921,8 +1385,22 @@
       <c r="F33">
         <v>27</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H33" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I33" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K33">
+        <v>68</v>
+      </c>
+      <c r="L33">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -936,8 +1414,22 @@
       <c r="F34">
         <v>26</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H34" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I34" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K34">
+        <v>69</v>
+      </c>
+      <c r="L34">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -951,8 +1443,22 @@
       <c r="F35">
         <v>42</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H35">
+        <f t="shared" si="3"/>
+        <v>34</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="4"/>
+        <v>42</v>
+      </c>
+      <c r="K35">
+        <v>70</v>
+      </c>
+      <c r="L35">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -966,8 +1472,22 @@
       <c r="F36">
         <v>41</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H36">
+        <f t="shared" si="3"/>
+        <v>35</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="4"/>
+        <v>41</v>
+      </c>
+      <c r="K36">
+        <v>71</v>
+      </c>
+      <c r="L36">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -981,8 +1501,22 @@
       <c r="F37">
         <v>40</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H37">
+        <f t="shared" si="3"/>
+        <v>36</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="K37">
+        <v>77</v>
+      </c>
+      <c r="L37">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -996,8 +1530,22 @@
       <c r="F38">
         <v>39</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H38">
+        <f t="shared" si="3"/>
+        <v>37</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="4"/>
+        <v>39</v>
+      </c>
+      <c r="K38">
+        <v>78</v>
+      </c>
+      <c r="L38">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -1008,8 +1556,22 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H39" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I39" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K39">
+        <v>79</v>
+      </c>
+      <c r="L39">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -1023,8 +1585,22 @@
       <c r="F40">
         <v>37</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H40" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I40" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K40">
+        <v>80</v>
+      </c>
+      <c r="L40">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -1038,8 +1614,22 @@
       <c r="F41">
         <v>36</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H41" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I41" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K41">
+        <v>85</v>
+      </c>
+      <c r="L41">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -1053,8 +1643,22 @@
       <c r="F42">
         <v>35</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H42" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I42" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K42">
+        <v>88</v>
+      </c>
+      <c r="L42">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -1068,8 +1672,22 @@
       <c r="F43">
         <v>34</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H43" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I43" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K43">
+        <v>90</v>
+      </c>
+      <c r="L43">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -1083,8 +1701,22 @@
       <c r="F44">
         <v>50</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H44">
+        <f t="shared" si="3"/>
+        <v>43</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="4"/>
+        <v>50</v>
+      </c>
+      <c r="K44">
+        <v>93</v>
+      </c>
+      <c r="L44">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -1098,8 +1730,22 @@
       <c r="F45">
         <v>49</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H45">
+        <f t="shared" si="3"/>
+        <v>44</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="4"/>
+        <v>49</v>
+      </c>
+      <c r="K45">
+        <v>95</v>
+      </c>
+      <c r="L45">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -1113,8 +1759,22 @@
       <c r="F46">
         <v>48</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H46">
+        <f t="shared" si="3"/>
+        <v>45</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="4"/>
+        <v>48</v>
+      </c>
+      <c r="K46">
+        <v>98</v>
+      </c>
+      <c r="L46">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -1128,8 +1788,22 @@
       <c r="F47">
         <v>47</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H47">
+        <f t="shared" si="3"/>
+        <v>46</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="4"/>
+        <v>47</v>
+      </c>
+      <c r="K47">
+        <v>100</v>
+      </c>
+      <c r="L47">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -1143,8 +1817,22 @@
       <c r="F48">
         <v>46</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H48" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I48" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K48">
+        <v>103</v>
+      </c>
+      <c r="L48">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="49" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -1158,8 +1846,16 @@
       <c r="F49">
         <v>45</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H49" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I49" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -1173,8 +1869,16 @@
       <c r="F50">
         <v>44</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H50" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I50" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -1188,8 +1892,23 @@
       <c r="F51">
         <v>43</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H51" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I51" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K51" t="s">
+        <v>11</v>
+      </c>
+      <c r="L51" t="str">
+        <f>IF(E102=1,I102,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -1203,8 +1922,163 @@
       <c r="F52">
         <v>59</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H52">
+        <f t="shared" si="3"/>
+        <v>51</v>
+      </c>
+      <c r="I52">
+        <f t="shared" si="4"/>
+        <v>59</v>
+      </c>
+      <c r="K52" t="s">
+        <v>11</v>
+      </c>
+      <c r="L52" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M52">
+        <v>1</v>
+      </c>
+      <c r="N52">
+        <v>2</v>
+      </c>
+      <c r="O52">
+        <v>5</v>
+      </c>
+      <c r="P52">
+        <v>8</v>
+      </c>
+      <c r="Q52">
+        <v>10</v>
+      </c>
+      <c r="R52">
+        <v>13</v>
+      </c>
+      <c r="S52">
+        <v>14</v>
+      </c>
+      <c r="T52">
+        <v>15</v>
+      </c>
+      <c r="U52">
+        <v>19</v>
+      </c>
+      <c r="V52">
+        <v>20</v>
+      </c>
+      <c r="W52">
+        <v>21</v>
+      </c>
+      <c r="X52">
+        <v>26</v>
+      </c>
+      <c r="Y52">
+        <v>27</v>
+      </c>
+      <c r="Z52">
+        <v>28</v>
+      </c>
+      <c r="AA52">
+        <v>29</v>
+      </c>
+      <c r="AB52">
+        <v>34</v>
+      </c>
+      <c r="AC52">
+        <v>35</v>
+      </c>
+      <c r="AD52">
+        <v>36</v>
+      </c>
+      <c r="AE52">
+        <v>37</v>
+      </c>
+      <c r="AF52">
+        <v>43</v>
+      </c>
+      <c r="AG52">
+        <v>44</v>
+      </c>
+      <c r="AH52">
+        <v>45</v>
+      </c>
+      <c r="AI52">
+        <v>46</v>
+      </c>
+      <c r="AJ52">
+        <v>51</v>
+      </c>
+      <c r="AK52">
+        <v>52</v>
+      </c>
+      <c r="AL52">
+        <v>53</v>
+      </c>
+      <c r="AM52">
+        <v>54</v>
+      </c>
+      <c r="AN52">
+        <v>60</v>
+      </c>
+      <c r="AO52">
+        <v>61</v>
+      </c>
+      <c r="AP52">
+        <v>62</v>
+      </c>
+      <c r="AQ52">
+        <v>63</v>
+      </c>
+      <c r="AR52">
+        <v>68</v>
+      </c>
+      <c r="AS52">
+        <v>69</v>
+      </c>
+      <c r="AT52">
+        <v>70</v>
+      </c>
+      <c r="AU52">
+        <v>71</v>
+      </c>
+      <c r="AV52">
+        <v>77</v>
+      </c>
+      <c r="AW52">
+        <v>78</v>
+      </c>
+      <c r="AX52">
+        <v>79</v>
+      </c>
+      <c r="AY52">
+        <v>80</v>
+      </c>
+      <c r="AZ52">
+        <v>85</v>
+      </c>
+      <c r="BA52">
+        <v>88</v>
+      </c>
+      <c r="BB52">
+        <v>90</v>
+      </c>
+      <c r="BC52">
+        <v>93</v>
+      </c>
+      <c r="BD52">
+        <v>95</v>
+      </c>
+      <c r="BE52">
+        <v>98</v>
+      </c>
+      <c r="BF52">
+        <v>100</v>
+      </c>
+      <c r="BG52">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="53" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -1218,8 +2092,160 @@
       <c r="F53">
         <v>58</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H53">
+        <f t="shared" si="3"/>
+        <v>52</v>
+      </c>
+      <c r="I53">
+        <f t="shared" si="4"/>
+        <v>58</v>
+      </c>
+      <c r="L53" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M53">
+        <v>4</v>
+      </c>
+      <c r="N53">
+        <v>3</v>
+      </c>
+      <c r="O53">
+        <v>7</v>
+      </c>
+      <c r="P53">
+        <v>9</v>
+      </c>
+      <c r="Q53">
+        <v>12</v>
+      </c>
+      <c r="R53">
+        <v>18</v>
+      </c>
+      <c r="S53">
+        <v>17</v>
+      </c>
+      <c r="T53">
+        <v>16</v>
+      </c>
+      <c r="U53">
+        <v>25</v>
+      </c>
+      <c r="V53">
+        <v>24</v>
+      </c>
+      <c r="W53">
+        <v>23</v>
+      </c>
+      <c r="X53">
+        <v>33</v>
+      </c>
+      <c r="Y53">
+        <v>32</v>
+      </c>
+      <c r="Z53">
+        <v>31</v>
+      </c>
+      <c r="AA53">
+        <v>30</v>
+      </c>
+      <c r="AB53">
+        <v>42</v>
+      </c>
+      <c r="AC53">
+        <v>41</v>
+      </c>
+      <c r="AD53">
+        <v>40</v>
+      </c>
+      <c r="AE53">
+        <v>39</v>
+      </c>
+      <c r="AF53">
+        <v>50</v>
+      </c>
+      <c r="AG53">
+        <v>49</v>
+      </c>
+      <c r="AH53">
+        <v>48</v>
+      </c>
+      <c r="AI53">
+        <v>47</v>
+      </c>
+      <c r="AJ53">
+        <v>59</v>
+      </c>
+      <c r="AK53">
+        <v>58</v>
+      </c>
+      <c r="AL53">
+        <v>57</v>
+      </c>
+      <c r="AM53">
+        <v>56</v>
+      </c>
+      <c r="AN53">
+        <v>67</v>
+      </c>
+      <c r="AO53">
+        <v>66</v>
+      </c>
+      <c r="AP53">
+        <v>65</v>
+      </c>
+      <c r="AQ53">
+        <v>64</v>
+      </c>
+      <c r="AR53">
+        <v>76</v>
+      </c>
+      <c r="AS53">
+        <v>75</v>
+      </c>
+      <c r="AT53">
+        <v>74</v>
+      </c>
+      <c r="AU53">
+        <v>73</v>
+      </c>
+      <c r="AV53">
+        <v>84</v>
+      </c>
+      <c r="AW53">
+        <v>83</v>
+      </c>
+      <c r="AX53">
+        <v>82</v>
+      </c>
+      <c r="AY53">
+        <v>81</v>
+      </c>
+      <c r="AZ53">
+        <v>87</v>
+      </c>
+      <c r="BA53">
+        <v>89</v>
+      </c>
+      <c r="BB53">
+        <v>92</v>
+      </c>
+      <c r="BC53">
+        <v>94</v>
+      </c>
+      <c r="BD53">
+        <v>97</v>
+      </c>
+      <c r="BE53">
+        <v>99</v>
+      </c>
+      <c r="BF53">
+        <v>102</v>
+      </c>
+      <c r="BG53">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="54" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -1233,8 +2259,16 @@
       <c r="F54">
         <v>57</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H54">
+        <f t="shared" si="3"/>
+        <v>53</v>
+      </c>
+      <c r="I54">
+        <f t="shared" si="4"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="55" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -1248,8 +2282,16 @@
       <c r="F55">
         <v>56</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H55">
+        <f t="shared" si="3"/>
+        <v>54</v>
+      </c>
+      <c r="I55">
+        <f t="shared" si="4"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="56" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -1263,8 +2305,16 @@
       <c r="F56" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H56" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I56" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="57" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -1278,8 +2328,16 @@
       <c r="F57">
         <v>54</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H57" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I57" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -1293,8 +2351,16 @@
       <c r="F58">
         <v>53</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H58" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I58" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="59" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -1308,8 +2374,16 @@
       <c r="F59">
         <v>52</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H59" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I59" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="60" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -1323,8 +2397,16 @@
       <c r="F60">
         <v>51</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H60" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I60" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -1338,8 +2420,16 @@
       <c r="F61">
         <v>67</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H61">
+        <f t="shared" si="3"/>
+        <v>60</v>
+      </c>
+      <c r="I61">
+        <f t="shared" si="4"/>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="62" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -1353,8 +2443,16 @@
       <c r="F62">
         <v>66</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H62">
+        <f t="shared" si="3"/>
+        <v>61</v>
+      </c>
+      <c r="I62">
+        <f t="shared" si="4"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="63" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -1368,8 +2466,16 @@
       <c r="F63">
         <v>65</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H63">
+        <f t="shared" si="3"/>
+        <v>62</v>
+      </c>
+      <c r="I63">
+        <f t="shared" si="4"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="64" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -1383,8 +2489,16 @@
       <c r="F64">
         <v>64</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H64">
+        <f t="shared" si="3"/>
+        <v>63</v>
+      </c>
+      <c r="I64">
+        <f t="shared" si="4"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -1398,8 +2512,16 @@
       <c r="F65">
         <v>63</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H65" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I65" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -1413,8 +2535,16 @@
       <c r="F66">
         <v>62</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H66" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I66" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -1422,14 +2552,22 @@
         <v>1</v>
       </c>
       <c r="E67">
-        <f t="shared" ref="E67:E106" si="1">SUM(B67:D67)</f>
+        <f t="shared" ref="E67:E106" si="5">SUM(B67:D67)</f>
         <v>1</v>
       </c>
       <c r="F67">
         <v>61</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H67" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I67" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -1437,14 +2575,22 @@
         <v>1</v>
       </c>
       <c r="E68">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F68">
         <v>60</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H68" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I68" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -1452,14 +2598,22 @@
         <v>1</v>
       </c>
       <c r="E69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F69">
         <v>76</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H69">
+        <f t="shared" si="3"/>
+        <v>68</v>
+      </c>
+      <c r="I69">
+        <f t="shared" si="4"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -1467,14 +2621,22 @@
         <v>1</v>
       </c>
       <c r="E70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F70">
         <v>75</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H70">
+        <f t="shared" si="3"/>
+        <v>69</v>
+      </c>
+      <c r="I70">
+        <f t="shared" si="4"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -1482,14 +2644,22 @@
         <v>1</v>
       </c>
       <c r="E71">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F71">
         <v>74</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H71">
+        <f t="shared" si="3"/>
+        <v>70</v>
+      </c>
+      <c r="I71">
+        <f t="shared" si="4"/>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -1497,14 +2667,22 @@
         <v>1</v>
       </c>
       <c r="E72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F72">
         <v>73</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H72">
+        <f t="shared" si="3"/>
+        <v>71</v>
+      </c>
+      <c r="I72">
+        <f t="shared" si="4"/>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -1512,14 +2690,29 @@
         <v>1</v>
       </c>
       <c r="E73">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F73" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H73" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I73" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K73" t="s">
+        <v>11</v>
+      </c>
+      <c r="L73" t="str">
+        <f>IF(E100=1,I100,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -1527,14 +2720,22 @@
         <v>1</v>
       </c>
       <c r="E74">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F74">
         <v>71</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H74" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I74" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -1542,14 +2743,22 @@
         <v>1</v>
       </c>
       <c r="E75">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F75">
         <v>70</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H75" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I75" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -1557,14 +2766,22 @@
         <v>1</v>
       </c>
       <c r="E76">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F76">
         <v>69</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H76" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I76" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>76</v>
       </c>
@@ -1572,14 +2789,22 @@
         <v>1</v>
       </c>
       <c r="E77">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F77">
         <v>68</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H77" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I77" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>77</v>
       </c>
@@ -1587,14 +2812,22 @@
         <v>1</v>
       </c>
       <c r="E78">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F78">
         <v>84</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H78">
+        <f t="shared" si="3"/>
+        <v>77</v>
+      </c>
+      <c r="I78">
+        <f t="shared" si="4"/>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>78</v>
       </c>
@@ -1602,14 +2835,22 @@
         <v>1</v>
       </c>
       <c r="E79">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F79">
         <v>83</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H79">
+        <f t="shared" si="3"/>
+        <v>78</v>
+      </c>
+      <c r="I79">
+        <f t="shared" si="4"/>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>79</v>
       </c>
@@ -1617,14 +2858,22 @@
         <v>1</v>
       </c>
       <c r="E80">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F80">
         <v>82</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H80">
+        <f t="shared" si="3"/>
+        <v>79</v>
+      </c>
+      <c r="I80">
+        <f t="shared" si="4"/>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>80</v>
       </c>
@@ -1632,14 +2881,22 @@
         <v>1</v>
       </c>
       <c r="E81">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F81">
         <v>81</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H81">
+        <f t="shared" ref="H81:H106" si="6">IF(B81=1,A81,"")</f>
+        <v>80</v>
+      </c>
+      <c r="I81">
+        <f t="shared" ref="I81:I106" si="7">IF(B81=1,F81,"")</f>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>81</v>
       </c>
@@ -1647,14 +2904,22 @@
         <v>1</v>
       </c>
       <c r="E82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F82">
         <v>80</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H82" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I82" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>82</v>
       </c>
@@ -1662,14 +2927,22 @@
         <v>1</v>
       </c>
       <c r="E83">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F83">
         <v>79</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H83" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I83" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>83</v>
       </c>
@@ -1677,14 +2950,22 @@
         <v>1</v>
       </c>
       <c r="E84">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F84">
         <v>78</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H84" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I84" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>84</v>
       </c>
@@ -1692,14 +2973,22 @@
         <v>1</v>
       </c>
       <c r="E85">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F85">
         <v>77</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H85" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I85" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>85</v>
       </c>
@@ -1707,14 +2996,22 @@
         <v>1</v>
       </c>
       <c r="E86">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F86">
         <v>87</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H86">
+        <f t="shared" si="6"/>
+        <v>85</v>
+      </c>
+      <c r="I86">
+        <f t="shared" si="7"/>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>86</v>
       </c>
@@ -1722,14 +3019,22 @@
         <v>1</v>
       </c>
       <c r="E87">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F87" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H87" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I87" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>87</v>
       </c>
@@ -1737,14 +3042,22 @@
         <v>1</v>
       </c>
       <c r="E88">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F88">
         <v>85</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H88" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I88" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>88</v>
       </c>
@@ -1752,14 +3065,22 @@
         <v>1</v>
       </c>
       <c r="E89">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F89">
         <v>89</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H89">
+        <f t="shared" si="6"/>
+        <v>88</v>
+      </c>
+      <c r="I89">
+        <f t="shared" si="7"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>89</v>
       </c>
@@ -1767,14 +3088,22 @@
         <v>1</v>
       </c>
       <c r="E90">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F90">
         <v>88</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H90" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I90" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>90</v>
       </c>
@@ -1782,14 +3111,22 @@
         <v>1</v>
       </c>
       <c r="E91">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F91">
         <v>92</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H91">
+        <f t="shared" si="6"/>
+        <v>90</v>
+      </c>
+      <c r="I91">
+        <f t="shared" si="7"/>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>91</v>
       </c>
@@ -1797,14 +3134,22 @@
         <v>1</v>
       </c>
       <c r="E92">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F92" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H92" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I92" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>92</v>
       </c>
@@ -1812,14 +3157,22 @@
         <v>1</v>
       </c>
       <c r="E93">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F93">
         <v>90</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H93" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I93" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>93</v>
       </c>
@@ -1827,14 +3180,22 @@
         <v>1</v>
       </c>
       <c r="E94">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F94">
         <v>94</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H94">
+        <f t="shared" si="6"/>
+        <v>93</v>
+      </c>
+      <c r="I94">
+        <f t="shared" si="7"/>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>94</v>
       </c>
@@ -1842,14 +3203,22 @@
         <v>1</v>
       </c>
       <c r="E95">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F95">
         <v>93</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H95" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I95" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>95</v>
       </c>
@@ -1857,14 +3226,22 @@
         <v>1</v>
       </c>
       <c r="E96">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F96">
         <v>97</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H96">
+        <f t="shared" si="6"/>
+        <v>95</v>
+      </c>
+      <c r="I96">
+        <f t="shared" si="7"/>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>96</v>
       </c>
@@ -1872,14 +3249,22 @@
         <v>1</v>
       </c>
       <c r="E97">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F97" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H97" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I97" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>97</v>
       </c>
@@ -1887,14 +3272,22 @@
         <v>1</v>
       </c>
       <c r="E98">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F98">
         <v>95</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H98" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I98" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>98</v>
       </c>
@@ -1902,14 +3295,22 @@
         <v>1</v>
       </c>
       <c r="E99">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F99">
         <v>99</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H99">
+        <f t="shared" si="6"/>
+        <v>98</v>
+      </c>
+      <c r="I99">
+        <f t="shared" si="7"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>99</v>
       </c>
@@ -1917,14 +3318,22 @@
         <v>1</v>
       </c>
       <c r="E100">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F100">
         <v>98</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H100" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I100" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>100</v>
       </c>
@@ -1932,14 +3341,22 @@
         <v>1</v>
       </c>
       <c r="E101">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F101">
         <v>102</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H101">
+        <f t="shared" si="6"/>
+        <v>100</v>
+      </c>
+      <c r="I101">
+        <f t="shared" si="7"/>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>101</v>
       </c>
@@ -1947,14 +3364,22 @@
         <v>1</v>
       </c>
       <c r="E102">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F102" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H102" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I102" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>102</v>
       </c>
@@ -1962,14 +3387,22 @@
         <v>1</v>
       </c>
       <c r="E103">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F103">
         <v>100</v>
       </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H103" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I103" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>103</v>
       </c>
@@ -1977,14 +3410,22 @@
         <v>1</v>
       </c>
       <c r="E104">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F104">
         <v>104</v>
       </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H104">
+        <f t="shared" si="6"/>
+        <v>103</v>
+      </c>
+      <c r="I104">
+        <f t="shared" si="7"/>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>104</v>
       </c>
@@ -1992,14 +3433,22 @@
         <v>1</v>
       </c>
       <c r="E105">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F105">
         <v>103</v>
       </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H105" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I105" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>105</v>
       </c>
@@ -2007,11 +3456,19 @@
         <v>1</v>
       </c>
       <c r="E106">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F106" t="s">
         <v>6</v>
+      </c>
+      <c r="H106" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I106" t="str">
+        <f t="shared" si="7"/>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>